<commit_message>
add list of components сontinue
</commit_message>
<xml_diff>
--- a/Beer.xlsx
+++ b/Beer.xlsx
@@ -441,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:F15"/>
+  <dimension ref="B3:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,9 +452,10 @@
     <col min="2" max="2" width="34.7109375" customWidth="1"/>
     <col min="3" max="3" width="47.28515625" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="9" max="9" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -471,8 +472,11 @@
         <f>PRODUCT(D3,E3)</f>
         <v>5720</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I3" s="2">
+        <v>6866</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -490,7 +494,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -507,8 +511,11 @@
         <f t="shared" si="0"/>
         <v>270</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I5" s="2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -525,8 +532,11 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I6" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -544,7 +554,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -562,7 +572,7 @@
         <v>3040</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -580,7 +590,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>18</v>
       </c>
@@ -598,7 +608,7 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>10</v>
       </c>
@@ -616,7 +626,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>13</v>
       </c>
@@ -633,8 +643,11 @@
         <f t="shared" si="0"/>
         <v>909</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I12" s="2">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>20</v>
       </c>
@@ -652,7 +665,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>21</v>
       </c>
@@ -670,7 +683,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="F15">
         <f>SUM(F3:F14)</f>
         <v>12988</v>

</xml_diff>

<commit_message>
add items lo list payment
</commit_message>
<xml_diff>
--- a/Beer.xlsx
+++ b/Beer.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="81">
   <si>
     <t>Nextion Enhanced NX8048K070</t>
   </si>
@@ -244,6 +244,21 @@
   </si>
   <si>
     <t>Наклейки</t>
+  </si>
+  <si>
+    <t>SD карта</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вилка 32А </t>
+  </si>
+  <si>
+    <t>Розетка силовая</t>
+  </si>
+  <si>
+    <t>223 2P+N32A</t>
+  </si>
+  <si>
+    <t>523 2P + N 32А</t>
   </si>
 </sst>
 </file>
@@ -1032,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H28"/>
+  <dimension ref="B1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,8 +1065,8 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G1" s="2">
-        <f>SUM(G4:G35)</f>
-        <v>6812</v>
+        <f>SUM(G4:G39)</f>
+        <v>8271</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -1368,14 +1383,47 @@
       <c r="B26" t="s">
         <v>75</v>
       </c>
+      <c r="G26" s="2">
+        <v>333</v>
+      </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>73</v>
+        <v>76</v>
+      </c>
+      <c r="G27" s="2">
+        <v>500</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
+      <c r="G28" s="2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="2">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>